<commit_message>
Update fix handling "special" whitepsace chars
</commit_message>
<xml_diff>
--- a/src/test/resources/spaces_data.xlsx
+++ b/src/test/resources/spaces_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradjacobs/git/bradjacobs/excel-to-csv/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631CEFEA-7710-5446-989B-FBBCE8348C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6C94F0-B8C4-224A-8244-FEBE495A127A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2460" windowWidth="26440" windowHeight="14600" xr2:uid="{10485244-3904-C643-B72B-40AF54D6D66F}"/>
+    <workbookView xWindow="1980" yWindow="2280" windowWidth="26440" windowHeight="14600" xr2:uid="{10485244-3904-C643-B72B-40AF54D6D66F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>HEADER_A</t>
   </si>
@@ -72,6 +72,105 @@
   </si>
   <si>
     <t xml:space="preserve">					</t>
+  </si>
+  <si>
+    <t>before_hair_space</t>
+  </si>
+  <si>
+    <t>after_hair_space</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>before_zero_width</t>
+  </si>
+  <si>
+    <t>after_zero_width</t>
+  </si>
+  <si>
+    <t>​</t>
+  </si>
+  <si>
+    <t>before_six-per-em</t>
+  </si>
+  <si>
+    <t>after_six-per-em</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>before_thin_space</t>
+  </si>
+  <si>
+    <t>after_thin_space</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>before_punctuation_space</t>
+  </si>
+  <si>
+    <t>after_punctuation_space</t>
+  </si>
+  <si>
+    <t>before_four-per-em</t>
+  </si>
+  <si>
+    <t>after_four-per-em</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>before_three-per-em</t>
+  </si>
+  <si>
+    <t>after_three-per-em</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>before_figure_space</t>
+  </si>
+  <si>
+    <t>after_figure_space</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>before_en_space</t>
+  </si>
+  <si>
+    <t>after_en_space</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>before_em_space</t>
+  </si>
+  <si>
+    <t>after_em_space</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>before_braille_blank</t>
+  </si>
+  <si>
+    <t>after_braille_blank</t>
+  </si>
+  <si>
+    <t>⠀</t>
+  </si>
+  <si>
+    <t> </t>
   </si>
 </sst>
 </file>
@@ -423,16 +522,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05663585-ABAD-7C4F-A589-E409BDE3B760}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -448,35 +547,156 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add unittests for whitespace sanitizer
</commit_message>
<xml_diff>
--- a/src/test/resources/spaces_data.xlsx
+++ b/src/test/resources/spaces_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradjacobs/git/bradjacobs/excel-to-csv/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6C94F0-B8C4-224A-8244-FEBE495A127A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149D8E18-9E41-FD4F-AF35-29F14E8281EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2280" windowWidth="26440" windowHeight="14600" xr2:uid="{10485244-3904-C643-B72B-40AF54D6D66F}"/>
+    <workbookView xWindow="1980" yWindow="2280" windowWidth="26440" windowHeight="14600" activeTab="1" xr2:uid="{10485244-3904-C643-B72B-40AF54D6D66F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LAST_COL_WHITESPACE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <t>HEADER_A</t>
   </si>
@@ -524,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05663585-ABAD-7C4F-A589-E409BDE3B760}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -702,4 +703,139 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DAE02C-7A55-E141-A38D-99E3E4F03D81}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
zero-width space shouldn't be counted as space for replacement
</commit_message>
<xml_diff>
--- a/src/test/resources/spaces_data.xlsx
+++ b/src/test/resources/spaces_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradjacobs/git/bradjacobs/excel-to-csv/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149D8E18-9E41-FD4F-AF35-29F14E8281EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E20D90D-8A79-C046-98B1-E813BB38CF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2280" windowWidth="26440" windowHeight="14600" activeTab="1" xr2:uid="{10485244-3904-C643-B72B-40AF54D6D66F}"/>
+    <workbookView xWindow="1980" yWindow="2280" windowWidth="26440" windowHeight="14600" xr2:uid="{10485244-3904-C643-B72B-40AF54D6D66F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
   <si>
     <t>HEADER_A</t>
   </si>
@@ -82,15 +82,6 @@
   </si>
   <si>
     <t> </t>
-  </si>
-  <si>
-    <t>before_zero_width</t>
-  </si>
-  <si>
-    <t>after_zero_width</t>
-  </si>
-  <si>
-    <t>​</t>
   </si>
   <si>
     <t>before_six-per-em</t>
@@ -227,9 +218,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -267,7 +258,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -373,7 +364,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -515,7 +506,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -523,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05663585-ABAD-7C4F-A589-E409BDE3B760}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,7 +608,7 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -625,13 +616,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -687,17 +678,6 @@
       </c>
       <c r="C14" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -707,10 +687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DAE02C-7A55-E141-A38D-99E3E4F03D81}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,15 +756,15 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -825,14 +805,6 @@
       </c>
       <c r="B14" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>